<commit_message>
Fixed some overflow and divide-by-zero errors.  Also fixed a weird bug with delimiters during text file opening
</commit_message>
<xml_diff>
--- a/Excel_Macros/Project_PopRecordings_Template.xlsx
+++ b/Excel_Macros/Project_PopRecordings_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Renna_Lab\Male Female stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dan_Programming\Programs\WaveAnalysisScripts\Excel_Macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
     <definedName name="TTTails">[1]Stats!$B$3</definedName>
     <definedName name="TTType">[1]Stats!$B$4</definedName>
   </definedNames>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -460,7 +460,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -486,6 +488,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
+      <c r="C2" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Removed all class IDs, except from Recordings, to make the Summary and PopRecordings spreadsheets more user friendly
</commit_message>
<xml_diff>
--- a/Excel_Macros/Project_PopRecordings_Template.xlsx
+++ b/Excel_Macros/Project_PopRecordings_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dan_Programming\Programs\WaveAnalysisScripts\Excel_Macros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\RennaLabSA1\Desktop\Dan's Folder\Git_Repos\WaveAnalysisScripts\Excel_Macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,13 +36,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Population ID</t>
-  </si>
-  <si>
     <t>Text File</t>
   </si>
   <si>
     <t>Recording ID</t>
+  </si>
+  <si>
+    <t>Population Name</t>
   </si>
 </sst>
 </file>
@@ -187,7 +187,7 @@
   <autoFilter ref="A1:C2"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Recording ID" dataDxfId="2"/>
-    <tableColumn id="3" name="Population ID" dataDxfId="1"/>
+    <tableColumn id="3" name="Population Name" dataDxfId="1"/>
     <tableColumn id="4" name="Text File" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -461,13 +461,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="108.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="52.5703125" style="2" customWidth="1"/>
@@ -476,13 +476,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Population info has been moved to the PopRecordings workbook, and WaveAnalyzeTextFiles has much better error handling during DefineObjects()
</commit_message>
<xml_diff>
--- a/Excel_Macros/Project_PopRecordings_Template.xlsx
+++ b/Excel_Macros/Project_PopRecordings_Template.xlsx
@@ -5,17 +5,18 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\RennaLabSA1\Desktop\Dan's Folder\Git_Repos\WaveAnalysisScripts\Excel_Macros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dan\WaveAnalysisScripts\Excel_Macros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
-    <sheet name="Recordings" sheetId="3" r:id="rId1"/>
+    <sheet name="Populations" sheetId="4" r:id="rId1"/>
+    <sheet name="Associated_Recordings" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="PropertyCols">[1]Figures!$A$4</definedName>
@@ -24,7 +25,7 @@
     <definedName name="TTTails">[1]Stats!$B$3</definedName>
     <definedName name="TTType">[1]Stats!$B$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,21 +35,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Text File</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Recording ID</t>
   </si>
   <si>
-    <t>Population Name</t>
+    <t>Control?</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Associated Population Name</t>
+  </si>
+  <si>
+    <t>Text File Path</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,7 +103,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -105,6 +115,21 @@
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -183,12 +208,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Recordings" displayName="Recordings" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Populations" displayName="Populations" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:C2"/>
+  <tableColumns count="3">
+    <tableColumn id="4" name="Name" dataDxfId="7"/>
+    <tableColumn id="3" name="Abbreviation" dataDxfId="6"/>
+    <tableColumn id="2" name="Control?" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Associated_Recordings" displayName="Associated_Recordings" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C2"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Recording ID" dataDxfId="2"/>
-    <tableColumn id="3" name="Population Name" dataDxfId="1"/>
-    <tableColumn id="4" name="Text File" dataDxfId="0"/>
+    <tableColumn id="3" name="Associated Population Name" dataDxfId="1"/>
+    <tableColumn id="4" name="Text File Path" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -457,17 +494,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="108.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="52.5703125" style="2" customWidth="1"/>
@@ -476,13 +554,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>